<commit_message>
[UPDATE] code converter csv to xl
</commit_message>
<xml_diff>
--- a/M1/solutions.xlsx
+++ b/M1/solutions.xlsx
@@ -345,7 +345,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>9,81</t>
+          <t>9.81</t>
         </is>
       </c>
     </row>
@@ -357,7 +357,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>16,09</t>
+          <t>16.09</t>
         </is>
       </c>
     </row>
@@ -369,7 +369,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>22,37</t>
+          <t>22.37</t>
         </is>
       </c>
     </row>
@@ -381,7 +381,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>28,65</t>
+          <t>28.65</t>
         </is>
       </c>
     </row>
@@ -393,7 +393,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>34,93</t>
+          <t>34.93</t>
         </is>
       </c>
     </row>
@@ -405,7 +405,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>41,21</t>
+          <t>41.21</t>
         </is>
       </c>
     </row>
@@ -417,7 +417,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>47,49</t>
+          <t>47.49</t>
         </is>
       </c>
     </row>
@@ -429,7 +429,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>53,77</t>
+          <t>53.77</t>
         </is>
       </c>
     </row>
@@ -441,7 +441,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>60,05</t>
+          <t>60.05</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>66,33</t>
+          <t>66.33</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>72,61</t>
+          <t>72.61</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>78,89</t>
+          <t>78.89</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>85,17</t>
+          <t>85.17</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>91,45</t>
+          <t>91.45</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>97,73</t>
+          <t>97.73</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>104,01</t>
+          <t>104.01</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>110,29</t>
+          <t>110.29</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>116,57</t>
+          <t>116.57</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>122,85</t>
+          <t>122.85</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>129,13</t>
+          <t>129.13</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>135,41</t>
+          <t>135.41</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>141,69</t>
+          <t>141.69</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>147,97</t>
+          <t>147.97</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>154,25</t>
+          <t>154.25</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>160,53</t>
+          <t>160.53</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>166,81</t>
+          <t>166.81</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>34,64</t>
+          <t>34.64</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>25,59</t>
+          <t>25.59</t>
         </is>
       </c>
     </row>
@@ -712,7 +712,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>28,52</t>
+          <t>28.52</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>40,42</t>
+          <t>40.42</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>11,12</t>
+          <t>11.12</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>61,20</t>
+          <t>61.20</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>44,10</t>
+          <t>44.10</t>
         </is>
       </c>
     </row>
@@ -772,7 +772,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>73,33</t>
+          <t>73.33</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>56,14</t>
+          <t>56.14</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>57,83</t>
+          <t>57.83</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>50,74</t>
+          <t>50.74</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>90,15</t>
+          <t>90.15</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>100,63</t>
+          <t>100.63</t>
         </is>
       </c>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>83,65</t>
+          <t>83.65</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>103,47</t>
+          <t>103.47</t>
         </is>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>89,48</t>
+          <t>89.48</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>128,12</t>
+          <t>128.12</t>
         </is>
       </c>
     </row>
@@ -892,7 +892,7 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>140,35</t>
+          <t>140.35</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>137,97</t>
+          <t>137.97</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>122,06</t>
+          <t>122.06</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>118,24</t>
+          <t>118.24</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>146,39</t>
+          <t>146.39</t>
         </is>
       </c>
     </row>
@@ -952,7 +952,7 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>138,15</t>
+          <t>138.15</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>158,85</t>
+          <t>158.85</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>135,65</t>
+          <t>135.65</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>187,84</t>
+          <t>187.84</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>-3,66</t>
+          <t>-3.66</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>93,89</t>
+          <t>93.89</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>3,04</t>
+          <t>3.04</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>202,57</t>
+          <t>202.57</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>217,01</t>
+          <t>217.01</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>287,28</t>
+          <t>287.28</t>
         </is>
       </c>
     </row>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>378,04</t>
+          <t>378.04</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>693,23</t>
+          <t>693.23</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>852,52</t>
+          <t>852.52</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>1005,74</t>
+          <t>1005.74</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>1202,23</t>
+          <t>1202.23</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>1559,58</t>
+          <t>1559.58</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>1911,75</t>
+          <t>1911.75</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>2142,29</t>
+          <t>2142.29</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>2519,12</t>
+          <t>2519.12</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>2799,50</t>
+          <t>2799.50</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>3148,96</t>
+          <t>3148.96</t>
         </is>
       </c>
     </row>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>3650,77</t>
+          <t>3650.77</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>4003,08</t>
+          <t>4003.08</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>4628,97</t>
+          <t>4628.97</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>5110,69</t>
+          <t>5110.69</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>5482,02</t>
+          <t>5482.02</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>6187,39</t>
+          <t>6187.39</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>6682,75</t>
+          <t>6682.75</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>7270,90</t>
+          <t>7270.90</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>7829,40</t>
+          <t>7829.40</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>67,85</t>
+          <t>67.85</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>35,37</t>
+          <t>35.37</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>27,60</t>
+          <t>27.60</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>32,37</t>
+          <t>32.37</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>95,57</t>
+          <t>95.57</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>65,69</t>
+          <t>65.69</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>53,22</t>
+          <t>53.22</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>72,80</t>
+          <t>72.80</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>6,83</t>
+          <t>6.83</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>39,99</t>
+          <t>39.99</t>
         </is>
       </c>
     </row>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>7,94</t>
+          <t>7.94</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>92,95</t>
+          <t>92.95</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>15,19</t>
+          <t>15.19</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>25,39</t>
+          <t>25.39</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>5,38</t>
+          <t>5.38</t>
         </is>
       </c>
     </row>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>10,83</t>
+          <t>10.83</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>38,88</t>
+          <t>38.88</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>77,00</t>
+          <t>77.00</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>56,19</t>
+          <t>56.19</t>
         </is>
       </c>
     </row>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>37,41</t>
+          <t>37.41</t>
         </is>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>25,80</t>
+          <t>25.80</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>90,98</t>
+          <t>90.98</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>50,51</t>
+          <t>50.51</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>18,94</t>
+          <t>18.94</t>
         </is>
       </c>
     </row>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>34,17</t>
+          <t>34.17</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>39,74</t>
+          <t>39.74</t>
         </is>
       </c>
     </row>

</xml_diff>